<commit_message>
working table creation and table entry from samples in trees_schema
</commit_message>
<xml_diff>
--- a/data/trees_schema.xlsx
+++ b/data/trees_schema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajay.anand/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajay.anand/Desktop/100KTrees_back/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6A2A54-28D1-5443-9792-6831AFDA245F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860B8A20-9F12-8049-8CD5-EC214BB44099}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="1" xr2:uid="{2C5A05E2-F556-6342-974C-0E66783C00A4}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="3" xr2:uid="{2C5A05E2-F556-6342-974C-0E66783C00A4}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="132">
   <si>
     <t>tree_id</t>
   </si>
@@ -119,9 +119,6 @@
     <t>user_zip</t>
   </si>
   <si>
-    <t>photo_id</t>
-  </si>
-  <si>
     <t>trees</t>
   </si>
   <si>
@@ -203,21 +200,6 @@
     <t>user_photo_html</t>
   </si>
   <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
     <t>tree_photo_html</t>
   </si>
   <si>
@@ -263,14 +245,200 @@
     <t>VARCHAR(255)</t>
   </si>
   <si>
-    <t>float8</t>
+    <t>Tree1</t>
+  </si>
+  <si>
+    <t>Tree2</t>
+  </si>
+  <si>
+    <t>Tree3</t>
+  </si>
+  <si>
+    <t>Tree4</t>
+  </si>
+  <si>
+    <t>Tree5</t>
+  </si>
+  <si>
+    <t>Tree6</t>
+  </si>
+  <si>
+    <t>Scientific Name 1</t>
+  </si>
+  <si>
+    <t>Scientific Name 2</t>
+  </si>
+  <si>
+    <t>Scientific Name 3</t>
+  </si>
+  <si>
+    <t>Alameda</t>
+  </si>
+  <si>
+    <t>2220 Buena Vista Ave</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>1755 Broadway</t>
+  </si>
+  <si>
+    <t>Oakland</t>
+  </si>
+  <si>
+    <t>1925 Webster St</t>
+  </si>
+  <si>
+    <t>1180 14th St</t>
+  </si>
+  <si>
+    <t>4465 S Larwin Ave</t>
+  </si>
+  <si>
+    <t>Concord</t>
+  </si>
+  <si>
+    <t>1459 Creekside Dr</t>
+  </si>
+  <si>
+    <t>Walnut Creek</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>image1 address</t>
+  </si>
+  <si>
+    <t>image2 address</t>
+  </si>
+  <si>
+    <t>image3 address</t>
+  </si>
+  <si>
+    <t>image4 address</t>
+  </si>
+  <si>
+    <t>image5 address</t>
+  </si>
+  <si>
+    <t>image6 address</t>
+  </si>
+  <si>
+    <t>Watered</t>
+  </si>
+  <si>
+    <t>Planted</t>
+  </si>
+  <si>
+    <t>someone1@gmail.com</t>
+  </si>
+  <si>
+    <t>someone2@gmail.com</t>
+  </si>
+  <si>
+    <t>someone3@gmail.com</t>
+  </si>
+  <si>
+    <t>someone4@gmail.com</t>
+  </si>
+  <si>
+    <t>someone5@gmail.com</t>
+  </si>
+  <si>
+    <t>someone6@gmail.com</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>password2</t>
+  </si>
+  <si>
+    <t>password3</t>
+  </si>
+  <si>
+    <t>password4</t>
+  </si>
+  <si>
+    <t>password5</t>
+  </si>
+  <si>
+    <t>password6</t>
+  </si>
+  <si>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>Name1</t>
+  </si>
+  <si>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>Name3</t>
+  </si>
+  <si>
+    <t>Name4</t>
+  </si>
+  <si>
+    <t>Name5</t>
+  </si>
+  <si>
+    <t>Name6</t>
+  </si>
+  <si>
+    <t>PhotoLink1</t>
+  </si>
+  <si>
+    <t>PhotoLink2</t>
+  </si>
+  <si>
+    <t>PhotoLink3</t>
+  </si>
+  <si>
+    <t>PhotoLink4</t>
+  </si>
+  <si>
+    <t>PhotoLink5</t>
+  </si>
+  <si>
+    <t>PhotoLink6</t>
+  </si>
+  <si>
+    <t>FLOAT8</t>
+  </si>
+  <si>
+    <t>TIMESTAMP</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -283,6 +451,33 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="32"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -302,14 +497,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -622,453 +825,559 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049435EF-C827-D146-8493-8D25FDD6A806}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
       <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" t="s">
-        <v>71</v>
+      <c r="E32" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1080,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7786DA17-9878-904B-9DA3-670D725ECDA7}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1092,8 +1401,8 @@
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.83203125" bestFit="1" customWidth="1"/>
@@ -1102,7 +1411,7 @@
     <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -1159,25 +1468,326 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2">
+        <v>37.779899999999998</v>
+      </c>
+      <c r="F2">
+        <v>-122.2822</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2">
+        <v>94501</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4">
+        <v>43831</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3">
+        <v>37.779091000000001</v>
+      </c>
+      <c r="F3">
+        <v>-122.276894</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3">
+        <v>94501</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <v>43832</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4">
+        <v>37.807560000000002</v>
+      </c>
+      <c r="F4">
+        <v>-122.26967</v>
+      </c>
+      <c r="G4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4">
+        <v>94612</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <v>43833</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5">
+        <v>37.809649999999998</v>
+      </c>
+      <c r="F5">
+        <v>-122.28653</v>
+      </c>
+      <c r="G5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5">
+        <v>94607</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>91</v>
+      </c>
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <v>43833</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6">
+        <v>37.948639999999997</v>
+      </c>
+      <c r="F6">
+        <v>-121.98733</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6">
+        <v>94521</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>92</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4">
+        <v>43834</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7">
+        <v>37.901760000000003</v>
+      </c>
+      <c r="F7">
+        <v>-122.06192</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7">
+        <v>94596</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>93</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <v>43834</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="40" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -1234,7 +1844,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1260,69 +1870,267 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="4">
+        <v>43831</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="4">
+        <v>43834</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="4">
+        <v>43840</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="4">
+        <v>43832</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="4">
+        <v>43840</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="4">
+        <v>43842</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="6">
+        <v>43833</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="4">
+        <v>43839</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="4">
+        <v>43840</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="4">
+        <v>43833</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="4">
+        <v>43845</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="4">
+        <v>43846</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="4">
+        <v>43834</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="4">
+        <v>43842</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="4">
+        <v>43850</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="4">
+        <v>43834</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="4">
+        <v>43855</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="4">
+        <v>43859</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
     </row>
   </sheetData>
@@ -1332,26 +2140,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032D1451-EFFC-644B-BD56-7EA48945AAB3}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1361,35 +2170,229 @@
       <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D4" s="1"/>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2">
+        <v>94612</v>
+      </c>
+      <c r="I2" s="4">
+        <v>43831</v>
+      </c>
+      <c r="J2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3">
+        <v>94501</v>
+      </c>
+      <c r="I3" s="4">
+        <v>43831</v>
+      </c>
+      <c r="J3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4">
+        <v>94521</v>
+      </c>
+      <c r="I4" s="4">
+        <v>43831</v>
+      </c>
+      <c r="J4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5">
+        <v>94507</v>
+      </c>
+      <c r="I5" s="4">
+        <v>43831</v>
+      </c>
+      <c r="J5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6">
+        <v>94607</v>
+      </c>
+      <c r="I6" s="4">
+        <v>43831</v>
+      </c>
+      <c r="J6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7">
+        <v>94607</v>
+      </c>
+      <c r="I7" s="4">
+        <v>43831</v>
+      </c>
+      <c r="J7" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4868FBCE-8812-8C4A-987D-7724E77F2F19}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{337F1ABB-8A98-9146-B6C8-DE10108A52CC}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{EA55E176-BE87-3F47-BD82-9DBEB8A1ECCE}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{239995AD-93D7-F742-B8ED-61E9955B79F8}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{860711E2-8820-9844-9B17-BFE2904CC049}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{D62EBF75-3A04-3C4F-B3E6-552CDF06C0E5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
creating the user log table
</commit_message>
<xml_diff>
--- a/data/trees_schema.xlsx
+++ b/data/trees_schema.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajay.anand/Desktop/100KTrees_back/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860B8A20-9F12-8049-8CD5-EC214BB44099}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C8E35F-41CA-0B4A-9B3B-25CF1959CCE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="3" xr2:uid="{2C5A05E2-F556-6342-974C-0E66783C00A4}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="4" xr2:uid="{2C5A05E2-F556-6342-974C-0E66783C00A4}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="6" r:id="rId1"/>
     <sheet name="trees" sheetId="1" r:id="rId2"/>
     <sheet name="trees_history" sheetId="2" r:id="rId3"/>
     <sheet name="users" sheetId="3" r:id="rId4"/>
+    <sheet name="user_log" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="134">
   <si>
     <t>tree_id</t>
   </si>
@@ -432,6 +433,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>user_login_time</t>
+  </si>
+  <si>
+    <t>user_logout_time</t>
   </si>
 </sst>
 </file>
@@ -2142,7 +2149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032D1451-EFFC-644B-BD56-7EA48945AAB3}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -2395,4 +2402,35 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6FCDA2-A672-8842-94D8-AF6E68F64783}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
trees_schema change to dictionary to add the users log table
</commit_message>
<xml_diff>
--- a/data/trees_schema.xlsx
+++ b/data/trees_schema.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajay.anand/Desktop/100KTrees_back/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C8E35F-41CA-0B4A-9B3B-25CF1959CCE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14A0D0D-4238-7F48-8949-257FFE58EE6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="4" xr2:uid="{2C5A05E2-F556-6342-974C-0E66783C00A4}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{2C5A05E2-F556-6342-974C-0E66783C00A4}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="6" r:id="rId1"/>
     <sheet name="trees" sheetId="1" r:id="rId2"/>
     <sheet name="trees_history" sheetId="2" r:id="rId3"/>
     <sheet name="users" sheetId="3" r:id="rId4"/>
-    <sheet name="user_log" sheetId="7" r:id="rId5"/>
+    <sheet name="users_log" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="139">
   <si>
     <t>tree_id</t>
   </si>
@@ -439,6 +439,21 @@
   </si>
   <si>
     <t>user_logout_time</t>
+  </si>
+  <si>
+    <t>users_log</t>
+  </si>
+  <si>
+    <t>user name</t>
+  </si>
+  <si>
+    <t>user id</t>
+  </si>
+  <si>
+    <t>user login time</t>
+  </si>
+  <si>
+    <t>user logout time</t>
   </si>
 </sst>
 </file>
@@ -832,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049435EF-C827-D146-8493-8D25FDD6A806}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1264,6 +1279,9 @@
       <c r="C25" t="s">
         <v>68</v>
       </c>
+      <c r="D25" t="s">
+        <v>135</v>
+      </c>
       <c r="E25" t="s">
         <v>131</v>
       </c>
@@ -1384,6 +1402,57 @@
         <v>65</v>
       </c>
       <c r="E32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2408,8 +2477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6FCDA2-A672-8842-94D8-AF6E68F64783}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>